<commit_message>
updating units & deviance explained
</commit_message>
<xml_diff>
--- a/data/Data LA Study 20220209.xlsx
+++ b/data/Data LA Study 20220209.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub22\La_wui\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D429E063-9832-4A0A-A036-112FB9F72263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D859CC9-9073-429C-AD21-E82690340DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_20220209_RForest" sheetId="10" r:id="rId1"/>
@@ -1825,121 +1825,7 @@
     <t xml:space="preserve">Type of the parcel use </t>
   </si>
   <si>
-    <t>Percent built land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent built land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent grass land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent paved land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent road land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent shrub land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent soil land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent tree land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 10 m around building</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 100 m around building</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 200 m around building</t>
-  </si>
-  <si>
-    <t>Percent water land cover, 300 m around building</t>
-  </si>
-  <si>
-    <t>Distance to nearest shrub (UNITS)</t>
-  </si>
-  <si>
-    <t>Distance to nearest tree (UNITS)</t>
-  </si>
-  <si>
     <t>Average height of trees overhanging building (UNITS)</t>
-  </si>
-  <si>
-    <t>Euclidian distance to any road (major and minor)- (UNITS)</t>
-  </si>
-  <si>
-    <t>Euclidian distance to major road (UNITS)</t>
-  </si>
-  <si>
-    <t>Elevation, 100 m around building, derived from a 30 m digital elevation model UNITS</t>
-  </si>
-  <si>
-    <t>Elevation, 30 m around building, derived from a 30 m digital elevation model UNITS</t>
   </si>
   <si>
     <r>
@@ -1998,6 +1884,120 @@
   </si>
   <si>
     <t>Does the building have DINS data (0,1)</t>
+  </si>
+  <si>
+    <t>Elevation, 100 m around building, derived from a 30 m digital elevation model (ft)</t>
+  </si>
+  <si>
+    <t>Elevation, 30 m around building, derived from a 30 m digital elevation model (ft)</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent built land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent grass land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent paved land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent road land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent shrub land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent soil land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent tree land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 10 ft around building</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 100 ft around building</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 200 ft around building</t>
+  </si>
+  <si>
+    <t>Percent water land cover, 300 ft around building</t>
+  </si>
+  <si>
+    <t>Euclidian distance to any road (major and minor) (m)</t>
+  </si>
+  <si>
+    <t>Euclidian distance to major road (m)</t>
+  </si>
+  <si>
+    <t>Distance to nearest shrub (ft)</t>
+  </si>
+  <si>
+    <t>Distance to nearest tree (ft)</t>
   </si>
 </sst>
 </file>
@@ -2268,7 +2268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2393,11 +2393,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2413,6 +2408,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2733,7 +2734,9 @@
   </sheetPr>
   <dimension ref="A1:K1015"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2758,7 +2761,7 @@
       <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="65" t="s">
         <v>481</v>
       </c>
       <c r="E1" s="59" t="s">
@@ -2790,11 +2793,11 @@
       <c r="C2" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="66" t="s">
         <v>483</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>627</v>
+        <v>589</v>
       </c>
       <c r="F2" s="54" t="s">
         <v>11</v>
@@ -2816,7 +2819,7 @@
       <c r="C3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="67" t="s">
         <v>484</v>
       </c>
       <c r="E3" s="63" t="s">
@@ -2842,7 +2845,7 @@
       <c r="C4" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="67" t="s">
         <v>485</v>
       </c>
       <c r="E4" s="63" t="s">
@@ -2868,7 +2871,7 @@
       <c r="C5" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="67" t="s">
         <v>486</v>
       </c>
       <c r="E5" s="63" t="s">
@@ -2894,7 +2897,7 @@
       <c r="C6" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="67" t="s">
         <v>487</v>
       </c>
       <c r="E6" s="63" t="s">
@@ -2920,7 +2923,7 @@
       <c r="C7" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="70" t="s">
+      <c r="D7" s="67" t="s">
         <v>488</v>
       </c>
       <c r="E7" s="63" t="s">
@@ -2946,7 +2949,7 @@
       <c r="C8" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="67" t="s">
         <v>489</v>
       </c>
       <c r="E8" s="61" t="s">
@@ -2972,7 +2975,7 @@
       <c r="C9" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="67" t="s">
         <v>490</v>
       </c>
       <c r="E9" s="63" t="s">
@@ -2998,7 +3001,7 @@
       <c r="C10" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="67" t="s">
         <v>491</v>
       </c>
       <c r="E10" s="63" t="s">
@@ -3024,7 +3027,7 @@
       <c r="C11" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="67" t="s">
         <v>492</v>
       </c>
       <c r="E11" s="63" t="s">
@@ -3050,7 +3053,7 @@
       <c r="C12" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="67" t="s">
         <v>493</v>
       </c>
       <c r="E12" s="63" t="s">
@@ -3076,7 +3079,7 @@
       <c r="C13" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="67" t="s">
         <v>495</v>
       </c>
       <c r="E13" s="63" t="s">
@@ -3103,11 +3106,11 @@
       <c r="C14" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="67" t="s">
         <v>496</v>
       </c>
-      <c r="E14" s="62" t="s">
-        <v>619</v>
+      <c r="E14" s="72" t="s">
+        <v>630</v>
       </c>
       <c r="F14" s="54" t="s">
         <v>11</v>
@@ -3130,11 +3133,11 @@
       <c r="C15" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="67" t="s">
         <v>497</v>
       </c>
-      <c r="E15" s="62" t="s">
-        <v>620</v>
+      <c r="E15" s="72" t="s">
+        <v>631</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>11</v>
@@ -3151,14 +3154,14 @@
       <c r="A16" s="52">
         <v>15</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="64" t="s">
         <v>463</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="70" t="s">
-        <v>629</v>
+      <c r="D16" s="67" t="s">
+        <v>591</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>554</v>
@@ -3186,11 +3189,11 @@
       <c r="C17" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="67" t="s">
         <v>498</v>
       </c>
       <c r="E17" s="62" t="s">
-        <v>621</v>
+        <v>587</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>11</v>
@@ -3213,7 +3216,7 @@
       <c r="C18" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D18" s="67" t="s">
         <v>499</v>
       </c>
       <c r="E18" s="63" t="s">
@@ -3242,7 +3245,7 @@
       <c r="C19" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="67" t="s">
         <v>500</v>
       </c>
       <c r="E19" s="63" t="s">
@@ -3271,7 +3274,7 @@
       <c r="C20" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="70" t="s">
+      <c r="D20" s="67" t="s">
         <v>501</v>
       </c>
       <c r="E20" s="63" t="s">
@@ -3298,7 +3301,7 @@
       <c r="C21" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="70" t="s">
+      <c r="D21" s="67" t="s">
         <v>502</v>
       </c>
       <c r="E21" s="63" t="s">
@@ -3325,7 +3328,7 @@
       <c r="C22" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D22" s="67" t="s">
         <v>503</v>
       </c>
       <c r="E22" s="63" t="s">
@@ -3352,7 +3355,7 @@
       <c r="C23" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="70" t="s">
+      <c r="D23" s="67" t="s">
         <v>504</v>
       </c>
       <c r="E23" s="61" t="s">
@@ -3379,7 +3382,7 @@
       <c r="C24" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="70" t="s">
+      <c r="D24" s="67" t="s">
         <v>505</v>
       </c>
       <c r="E24" s="61" t="s">
@@ -3406,7 +3409,7 @@
       <c r="C25" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="70" t="s">
+      <c r="D25" s="67" t="s">
         <v>506</v>
       </c>
       <c r="E25" s="63" t="s">
@@ -3433,7 +3436,7 @@
       <c r="C26" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="70" t="s">
+      <c r="D26" s="67" t="s">
         <v>507</v>
       </c>
       <c r="E26" s="61" t="s">
@@ -3462,7 +3465,7 @@
       <c r="C27" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="70" t="s">
+      <c r="D27" s="67" t="s">
         <v>508</v>
       </c>
       <c r="E27" s="63" t="s">
@@ -3488,7 +3491,7 @@
       <c r="C28" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="70" t="s">
+      <c r="D28" s="67" t="s">
         <v>494</v>
       </c>
       <c r="E28" s="63" t="s">
@@ -3514,11 +3517,11 @@
       <c r="C29" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="70" t="s">
+      <c r="D29" s="67" t="s">
         <v>509</v>
       </c>
       <c r="E29" s="62" t="s">
-        <v>628</v>
+        <v>590</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>11</v>
@@ -3544,7 +3547,7 @@
       <c r="C30" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="70" t="s">
+      <c r="D30" s="67" t="s">
         <v>543</v>
       </c>
       <c r="E30" s="62" t="s">
@@ -3572,11 +3575,11 @@
       <c r="C31" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="70" t="s">
+      <c r="D31" s="67" t="s">
         <v>544</v>
       </c>
-      <c r="E31" s="62" t="s">
-        <v>622</v>
+      <c r="E31" s="72" t="s">
+        <v>628</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>55</v>
@@ -3598,11 +3601,11 @@
       <c r="C32" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D32" s="70" t="s">
+      <c r="D32" s="67" t="s">
         <v>545</v>
       </c>
-      <c r="E32" s="62" t="s">
-        <v>623</v>
+      <c r="E32" s="72" t="s">
+        <v>629</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>55</v>
@@ -3623,11 +3626,11 @@
       <c r="C33" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="70" t="s">
+      <c r="D33" s="67" t="s">
         <v>510</v>
       </c>
       <c r="E33" s="63" t="s">
-        <v>587</v>
+        <v>596</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>11</v>
@@ -3650,11 +3653,11 @@
       <c r="C34" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="70" t="s">
+      <c r="D34" s="67" t="s">
         <v>511</v>
       </c>
       <c r="E34" s="63" t="s">
-        <v>588</v>
+        <v>597</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>11</v>
@@ -3675,11 +3678,11 @@
       <c r="C35" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D35" s="70" t="s">
+      <c r="D35" s="67" t="s">
         <v>512</v>
       </c>
       <c r="E35" s="63" t="s">
-        <v>589</v>
+        <v>598</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>11</v>
@@ -3700,11 +3703,11 @@
       <c r="C36" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="70" t="s">
+      <c r="D36" s="67" t="s">
         <v>513</v>
       </c>
       <c r="E36" s="63" t="s">
-        <v>590</v>
+        <v>599</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>11</v>
@@ -3725,11 +3728,11 @@
       <c r="C37" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="70" t="s">
+      <c r="D37" s="67" t="s">
         <v>514</v>
       </c>
       <c r="E37" s="63" t="s">
-        <v>591</v>
+        <v>600</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>11</v>
@@ -3750,11 +3753,11 @@
       <c r="C38" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="70" t="s">
+      <c r="D38" s="67" t="s">
         <v>515</v>
       </c>
       <c r="E38" s="61" t="s">
-        <v>592</v>
+        <v>601</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>11</v>
@@ -3775,11 +3778,11 @@
       <c r="C39" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="70" t="s">
+      <c r="D39" s="67" t="s">
         <v>516</v>
       </c>
       <c r="E39" s="61" t="s">
-        <v>593</v>
+        <v>602</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>11</v>
@@ -3800,11 +3803,11 @@
       <c r="C40" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="70" t="s">
+      <c r="D40" s="67" t="s">
         <v>517</v>
       </c>
       <c r="E40" s="61" t="s">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>11</v>
@@ -3825,11 +3828,11 @@
       <c r="C41" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D41" s="70" t="s">
+      <c r="D41" s="67" t="s">
         <v>518</v>
       </c>
       <c r="E41" s="61" t="s">
-        <v>595</v>
+        <v>604</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>11</v>
@@ -3850,11 +3853,11 @@
       <c r="C42" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D42" s="70" t="s">
+      <c r="D42" s="67" t="s">
         <v>519</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>596</v>
+        <v>605</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>11</v>
@@ -3875,11 +3878,11 @@
       <c r="C43" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="70" t="s">
+      <c r="D43" s="67" t="s">
         <v>520</v>
       </c>
       <c r="E43" s="61" t="s">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>11</v>
@@ -3900,11 +3903,11 @@
       <c r="C44" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D44" s="70" t="s">
+      <c r="D44" s="67" t="s">
         <v>521</v>
       </c>
       <c r="E44" s="61" t="s">
-        <v>598</v>
+        <v>607</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>11</v>
@@ -3926,11 +3929,11 @@
       <c r="C45" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="70" t="s">
+      <c r="D45" s="67" t="s">
         <v>522</v>
       </c>
       <c r="E45" s="61" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>11</v>
@@ -3953,11 +3956,11 @@
       <c r="C46" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="70" t="s">
+      <c r="D46" s="67" t="s">
         <v>523</v>
       </c>
       <c r="E46" s="61" t="s">
-        <v>600</v>
+        <v>609</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>11</v>
@@ -3980,11 +3983,11 @@
       <c r="C47" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="70" t="s">
+      <c r="D47" s="67" t="s">
         <v>524</v>
       </c>
       <c r="E47" s="61" t="s">
-        <v>601</v>
+        <v>610</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>11</v>
@@ -4007,11 +4010,11 @@
       <c r="C48" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="70" t="s">
+      <c r="D48" s="67" t="s">
         <v>525</v>
       </c>
       <c r="E48" s="61" t="s">
-        <v>602</v>
+        <v>611</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>11</v>
@@ -4034,11 +4037,11 @@
       <c r="C49" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="70" t="s">
+      <c r="D49" s="67" t="s">
         <v>526</v>
       </c>
       <c r="E49" s="61" t="s">
-        <v>603</v>
+        <v>612</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>11</v>
@@ -4061,11 +4064,11 @@
       <c r="C50" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="70" t="s">
+      <c r="D50" s="67" t="s">
         <v>527</v>
       </c>
       <c r="E50" s="61" t="s">
-        <v>604</v>
+        <v>613</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>11</v>
@@ -4088,11 +4091,11 @@
       <c r="C51" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="70" t="s">
+      <c r="D51" s="67" t="s">
         <v>528</v>
       </c>
       <c r="E51" s="61" t="s">
-        <v>605</v>
+        <v>614</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>11</v>
@@ -4115,11 +4118,11 @@
       <c r="C52" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D52" s="70" t="s">
+      <c r="D52" s="67" t="s">
         <v>529</v>
       </c>
       <c r="E52" s="61" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>11</v>
@@ -4142,11 +4145,11 @@
       <c r="C53" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D53" s="70" t="s">
+      <c r="D53" s="67" t="s">
         <v>530</v>
       </c>
       <c r="E53" s="61" t="s">
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>11</v>
@@ -4169,11 +4172,11 @@
       <c r="C54" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="70" t="s">
+      <c r="D54" s="67" t="s">
         <v>531</v>
       </c>
       <c r="E54" s="61" t="s">
-        <v>608</v>
+        <v>617</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>11</v>
@@ -4196,11 +4199,11 @@
       <c r="C55" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D55" s="70" t="s">
+      <c r="D55" s="67" t="s">
         <v>532</v>
       </c>
       <c r="E55" s="61" t="s">
-        <v>609</v>
+        <v>618</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>11</v>
@@ -4223,11 +4226,11 @@
       <c r="C56" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="70" t="s">
+      <c r="D56" s="67" t="s">
         <v>533</v>
       </c>
       <c r="E56" s="61" t="s">
-        <v>610</v>
+        <v>619</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>11</v>
@@ -4250,11 +4253,11 @@
       <c r="C57" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D57" s="70" t="s">
+      <c r="D57" s="67" t="s">
         <v>534</v>
       </c>
       <c r="E57" s="61" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>11</v>
@@ -4277,11 +4280,11 @@
       <c r="C58" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D58" s="70" t="s">
+      <c r="D58" s="67" t="s">
         <v>535</v>
       </c>
       <c r="E58" s="61" t="s">
-        <v>612</v>
+        <v>621</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>11</v>
@@ -4304,11 +4307,11 @@
       <c r="C59" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="70" t="s">
+      <c r="D59" s="67" t="s">
         <v>536</v>
       </c>
       <c r="E59" s="61" t="s">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>11</v>
@@ -4331,11 +4334,11 @@
       <c r="C60" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="70" t="s">
+      <c r="D60" s="67" t="s">
         <v>537</v>
       </c>
       <c r="E60" s="61" t="s">
-        <v>614</v>
+        <v>623</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>11</v>
@@ -4358,11 +4361,11 @@
       <c r="C61" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="70" t="s">
+      <c r="D61" s="67" t="s">
         <v>538</v>
       </c>
       <c r="E61" s="63" t="s">
-        <v>615</v>
+        <v>624</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>11</v>
@@ -4385,11 +4388,11 @@
       <c r="C62" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D62" s="70" t="s">
+      <c r="D62" s="67" t="s">
         <v>539</v>
       </c>
       <c r="E62" s="63" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
       <c r="F62" s="54" t="s">
         <v>11</v>
@@ -4412,11 +4415,11 @@
       <c r="C63" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D63" s="70" t="s">
+      <c r="D63" s="67" t="s">
         <v>540</v>
       </c>
       <c r="E63" s="63" t="s">
-        <v>617</v>
+        <v>626</v>
       </c>
       <c r="F63" s="54" t="s">
         <v>11</v>
@@ -4439,11 +4442,11 @@
       <c r="C64" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D64" s="70" t="s">
+      <c r="D64" s="67" t="s">
         <v>541</v>
       </c>
       <c r="E64" s="63" t="s">
-        <v>618</v>
+        <v>627</v>
       </c>
       <c r="F64" s="54" t="s">
         <v>11</v>
@@ -4466,11 +4469,11 @@
       <c r="C65" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D65" s="70" t="s">
+      <c r="D65" s="67" t="s">
         <v>542</v>
       </c>
       <c r="E65" s="62" t="s">
-        <v>626</v>
+        <v>588</v>
       </c>
       <c r="F65" s="54" t="s">
         <v>41</v>
@@ -4492,11 +4495,11 @@
       <c r="C66" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="D66" s="70" t="s">
-        <v>630</v>
-      </c>
-      <c r="E66" s="69" t="s">
-        <v>631</v>
+      <c r="D66" s="67" t="s">
+        <v>592</v>
+      </c>
+      <c r="E66" s="66" t="s">
+        <v>593</v>
       </c>
       <c r="F66" s="54" t="s">
         <v>11</v>
@@ -4518,7 +4521,7 @@
       <c r="C67" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="D67" s="69" t="s">
+      <c r="D67" s="66" t="s">
         <v>467</v>
       </c>
       <c r="E67" s="9" t="s">
@@ -4547,7 +4550,7 @@
       <c r="C68" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="D68" s="69" t="s">
+      <c r="D68" s="66" t="s">
         <v>466</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -4574,7 +4577,7 @@
       <c r="C69" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="D69" s="69" t="s">
+      <c r="D69" s="66" t="s">
         <v>465</v>
       </c>
       <c r="E69" s="9" t="s">
@@ -4600,7 +4603,7 @@
       <c r="C70" s="52" t="s">
         <v>461</v>
       </c>
-      <c r="D70" s="69" t="s">
+      <c r="D70" s="66" t="s">
         <v>464</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -4627,7 +4630,7 @@
       <c r="C71" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="D71" s="71" t="s">
+      <c r="D71" s="68" t="s">
         <v>579</v>
       </c>
       <c r="E71" s="55" t="s">
@@ -4651,7 +4654,7 @@
       <c r="C72" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D72" s="71" t="s">
+      <c r="D72" s="68" t="s">
         <v>546</v>
       </c>
       <c r="E72" s="55" t="s">
@@ -4683,7 +4686,7 @@
       <c r="C73" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D73" s="71" t="s">
+      <c r="D73" s="68" t="s">
         <v>547</v>
       </c>
       <c r="E73" s="55" t="s">
@@ -4715,11 +4718,11 @@
       <c r="C74" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D74" s="71" t="s">
+      <c r="D74" s="68" t="s">
         <v>548</v>
       </c>
       <c r="E74" s="62" t="s">
-        <v>624</v>
+        <v>594</v>
       </c>
       <c r="F74" s="54" t="s">
         <v>11</v>
@@ -4747,11 +4750,11 @@
       <c r="C75" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D75" s="71" t="s">
+      <c r="D75" s="68" t="s">
         <v>549</v>
       </c>
       <c r="E75" s="62" t="s">
-        <v>625</v>
+        <v>595</v>
       </c>
       <c r="F75" s="54" t="s">
         <v>11</v>
@@ -4779,7 +4782,7 @@
       <c r="C76" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D76" s="71" t="s">
+      <c r="D76" s="68" t="s">
         <v>550</v>
       </c>
       <c r="E76" s="55" t="s">
@@ -4809,7 +4812,7 @@
       <c r="C77" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="71" t="s">
+      <c r="D77" s="68" t="s">
         <v>551</v>
       </c>
       <c r="E77" s="55" t="s">
@@ -11407,15 +11410,15 @@
     <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66" t="s">
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="65"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>

</xml_diff>

<commit_message>
units for predictor variables
</commit_message>
<xml_diff>
--- a/data/Data LA Study 20220209.xlsx
+++ b/data/Data LA Study 20220209.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub22\La_wui\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46EF7C54-357A-45F3-95DB-36FFA093AC94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAAAC98-28E3-4D52-93D5-675019D8852A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="630" windowWidth="38370" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_20220209_RForest" sheetId="10" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="crosswalk_research_guidelines_d" sheetId="8" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_20220209_RForest!$A$1:$K$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data_20220209_RForest!$A$1:$K$77</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">data_checklist_190514!$A$2:$AE$92</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Data_request_190524!$A$2:$AC$56</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Price_2021 categories'!$A$2:$E$91</definedName>
@@ -2268,7 +2268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2409,6 +2409,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2732,10 +2735,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K1015"/>
+  <dimension ref="A1:K1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2950,10 +2953,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="67" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F8" s="54" t="s">
         <v>11</v>
@@ -2976,10 +2979,10 @@
         <v>13</v>
       </c>
       <c r="D9" s="67" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="F9" s="54" t="s">
         <v>11</v>
@@ -3002,10 +3005,10 @@
         <v>13</v>
       </c>
       <c r="D10" s="67" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F10" s="54" t="s">
         <v>11</v>
@@ -3021,23 +3024,23 @@
       <c r="A11" s="52">
         <v>10</v>
       </c>
-      <c r="B11" s="52" t="s">
+      <c r="B11" s="10" t="s">
         <v>293</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="67" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>578</v>
+        <v>553</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G11" s="54" t="s">
-        <v>12</v>
+        <v>477</v>
       </c>
       <c r="H11" s="54"/>
       <c r="I11" s="54"/>
@@ -3048,22 +3051,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>293</v>
+        <v>463</v>
       </c>
       <c r="C12" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="67" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>574</v>
+        <v>555</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="54" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="H12" s="54"/>
       <c r="I12" s="54"/>
@@ -3080,10 +3083,10 @@
         <v>13</v>
       </c>
       <c r="D13" s="67" t="s">
-        <v>495</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>555</v>
+        <v>496</v>
+      </c>
+      <c r="E13" s="69" t="s">
+        <v>629</v>
       </c>
       <c r="F13" s="54" t="s">
         <v>11</v>
@@ -3107,10 +3110,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="67" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E14" s="69" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F14" s="54" t="s">
         <v>11</v>
@@ -3127,17 +3130,17 @@
       <c r="A15" s="52">
         <v>14</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="64" t="s">
         <v>463</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="64" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="67" t="s">
-        <v>497</v>
-      </c>
-      <c r="E15" s="69" t="s">
-        <v>630</v>
+        <v>590</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>554</v>
       </c>
       <c r="F15" s="54" t="s">
         <v>11</v>
@@ -3154,17 +3157,17 @@
       <c r="A16" s="52">
         <v>15</v>
       </c>
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="52" t="s">
         <v>463</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="67" t="s">
-        <v>590</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>554</v>
+        <v>498</v>
+      </c>
+      <c r="E16" s="62" t="s">
+        <v>631</v>
       </c>
       <c r="F16" s="54" t="s">
         <v>11</v>
@@ -3183,17 +3186,17 @@
       <c r="A17" s="52">
         <v>16</v>
       </c>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C17" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="67" t="s">
-        <v>498</v>
-      </c>
-      <c r="E17" s="62" t="s">
-        <v>631</v>
+        <v>510</v>
+      </c>
+      <c r="E17" s="71" t="s">
+        <v>595</v>
       </c>
       <c r="F17" s="54" t="s">
         <v>11</v>
@@ -3201,26 +3204,26 @@
       <c r="G17" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="54" t="s">
+        <v>471</v>
+      </c>
       <c r="K17" s="54"/>
     </row>
     <row r="18" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="52">
         <v>17</v>
       </c>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="67" t="s">
-        <v>499</v>
+        <v>514</v>
       </c>
       <c r="E18" s="63" t="s">
-        <v>556</v>
+        <v>599</v>
       </c>
       <c r="F18" s="54" t="s">
         <v>11</v>
@@ -3228,60 +3231,52 @@
       <c r="G18" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="54" t="s">
-        <v>471</v>
-      </c>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="54"/>
       <c r="K18" s="54"/>
     </row>
     <row r="19" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="52">
         <v>18</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D19" s="67" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="E19" s="63" t="s">
-        <v>562</v>
+        <v>603</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G19" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="54" t="s">
-        <v>472</v>
-      </c>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
+      <c r="H19" s="54"/>
       <c r="K19" s="54"/>
     </row>
     <row r="20" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="52">
         <v>19</v>
       </c>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C20" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D20" s="67" t="s">
-        <v>501</v>
+        <v>522</v>
       </c>
       <c r="E20" s="63" t="s">
-        <v>563</v>
+        <v>607</v>
       </c>
       <c r="F20" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G20" s="54" t="s">
         <v>34</v>
@@ -3295,20 +3290,20 @@
       <c r="A21" s="52">
         <v>20</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="67" t="s">
-        <v>502</v>
+        <v>526</v>
       </c>
       <c r="E21" s="63" t="s">
-        <v>564</v>
+        <v>611</v>
       </c>
       <c r="F21" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G21" s="54" t="s">
         <v>34</v>
@@ -3322,20 +3317,20 @@
       <c r="A22" s="52">
         <v>21</v>
       </c>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D22" s="67" t="s">
-        <v>503</v>
+        <v>530</v>
       </c>
       <c r="E22" s="63" t="s">
-        <v>565</v>
+        <v>615</v>
       </c>
       <c r="F22" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G22" s="54" t="s">
         <v>34</v>
@@ -3349,20 +3344,20 @@
       <c r="A23" s="52">
         <v>22</v>
       </c>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D23" s="67" t="s">
-        <v>504</v>
+        <v>534</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>561</v>
+        <v>619</v>
       </c>
       <c r="F23" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G23" s="54" t="s">
         <v>34</v>
@@ -3376,20 +3371,20 @@
       <c r="A24" s="52">
         <v>23</v>
       </c>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="67" t="s">
-        <v>505</v>
+        <v>538</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>560</v>
+        <v>623</v>
       </c>
       <c r="F24" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G24" s="54" t="s">
         <v>34</v>
@@ -3410,21 +3405,21 @@
         <v>13</v>
       </c>
       <c r="D25" s="67" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="E25" s="63" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F25" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G25" s="54" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="54"/>
-      <c r="I25" s="54" t="s">
-        <v>480</v>
-      </c>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
     </row>
     <row r="26" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="52">
@@ -3437,49 +3432,49 @@
         <v>13</v>
       </c>
       <c r="D26" s="67" t="s">
-        <v>507</v>
+        <v>489</v>
       </c>
       <c r="E26" s="61" t="s">
-        <v>558</v>
+        <v>573</v>
       </c>
       <c r="F26" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G26" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="H26" s="54"/>
+        <v>12</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>471</v>
+      </c>
       <c r="I26" s="54"/>
       <c r="J26" s="54"/>
-      <c r="K26" s="54" t="s">
-        <v>47</v>
-      </c>
+      <c r="K26" s="54"/>
     </row>
     <row r="27" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="52">
         <v>26</v>
       </c>
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="10" t="s">
         <v>463</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="67" t="s">
-        <v>508</v>
+        <v>491</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="F27" s="54" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="I27" s="54" t="s">
-        <v>480</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="H27" s="54"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
     </row>
     <row r="28" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="52">
@@ -3492,49 +3487,49 @@
         <v>13</v>
       </c>
       <c r="D28" s="67" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>553</v>
+        <v>562</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>41</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>477</v>
-      </c>
-      <c r="H28" s="54"/>
+        <v>34</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>472</v>
+      </c>
       <c r="I28" s="54"/>
       <c r="J28" s="54"/>
+      <c r="K28" s="54"/>
     </row>
     <row r="29" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="52">
         <v>28</v>
       </c>
       <c r="B29" s="52" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
       <c r="C29" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D29" s="67" t="s">
-        <v>509</v>
-      </c>
-      <c r="E29" s="62" t="s">
-        <v>589</v>
+        <v>501</v>
+      </c>
+      <c r="E29" s="70" t="s">
+        <v>563</v>
       </c>
       <c r="F29" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G29" s="54" t="s">
-        <v>473</v>
-      </c>
-      <c r="H29" s="54" t="s">
-        <v>482</v>
-      </c>
-      <c r="I29" s="54" t="s">
-        <v>474</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H29" s="54"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="54"/>
       <c r="K29" s="54"/>
     </row>
     <row r="30" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3542,27 +3537,26 @@
         <v>29</v>
       </c>
       <c r="B30" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C30" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="67" t="s">
-        <v>543</v>
-      </c>
-      <c r="E30" s="62" t="s">
-        <v>580</v>
+        <v>502</v>
+      </c>
+      <c r="E30" s="70" t="s">
+        <v>564</v>
       </c>
       <c r="F30" s="54" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G30" s="54" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="H30" s="54"/>
-      <c r="I30" s="54" t="s">
-        <v>59</v>
-      </c>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
       <c r="K30" s="54"/>
     </row>
     <row r="31" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3570,25 +3564,26 @@
         <v>30</v>
       </c>
       <c r="B31" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D31" s="67" t="s">
-        <v>544</v>
-      </c>
-      <c r="E31" s="69" t="s">
-        <v>627</v>
+        <v>503</v>
+      </c>
+      <c r="E31" s="70" t="s">
+        <v>565</v>
       </c>
       <c r="F31" s="54" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G31" s="54" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="H31" s="54"/>
       <c r="I31" s="54"/>
+      <c r="J31" s="54"/>
       <c r="K31" s="54"/>
     </row>
     <row r="32" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3596,24 +3591,26 @@
         <v>31</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C32" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D32" s="67" t="s">
-        <v>545</v>
-      </c>
-      <c r="E32" s="69" t="s">
-        <v>628</v>
+        <v>504</v>
+      </c>
+      <c r="E32" s="70" t="s">
+        <v>561</v>
       </c>
       <c r="F32" s="54" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
       <c r="K32" s="54"/>
     </row>
     <row r="33" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3621,26 +3618,26 @@
         <v>32</v>
       </c>
       <c r="B33" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="67" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E33" s="63" t="s">
-        <v>595</v>
+        <v>560</v>
       </c>
       <c r="F33" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G33" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="54" t="s">
-        <v>471</v>
-      </c>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
       <c r="K33" s="54"/>
     </row>
     <row r="34" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3648,99 +3645,111 @@
         <v>33</v>
       </c>
       <c r="B34" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C34" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D34" s="67" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="E34" s="63" t="s">
-        <v>596</v>
+        <v>559</v>
       </c>
       <c r="F34" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G34" s="54" t="s">
         <v>34</v>
       </c>
       <c r="H34" s="54"/>
-      <c r="K34" s="54"/>
+      <c r="I34" s="54" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="35" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="52">
         <v>34</v>
       </c>
       <c r="B35" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C35" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="67" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="E35" s="63" t="s">
-        <v>597</v>
+        <v>558</v>
       </c>
       <c r="F35" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G35" s="54" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="54"/>
-      <c r="K35" s="54"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="54"/>
+      <c r="K35" s="54" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="36" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="52">
         <v>35</v>
       </c>
       <c r="B36" s="52" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C36" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="67" t="s">
-        <v>513</v>
-      </c>
-      <c r="E36" s="63" t="s">
-        <v>598</v>
+        <v>508</v>
+      </c>
+      <c r="E36" s="72" t="s">
+        <v>557</v>
       </c>
       <c r="F36" s="54" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G36" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H36" s="54"/>
-      <c r="K36" s="54"/>
+      <c r="I36" s="54" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="37" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="52">
         <v>36</v>
       </c>
       <c r="B37" s="52" t="s">
-        <v>462</v>
+        <v>475</v>
       </c>
       <c r="C37" s="52" t="s">
         <v>13</v>
       </c>
       <c r="D37" s="67" t="s">
-        <v>514</v>
-      </c>
-      <c r="E37" s="63" t="s">
-        <v>599</v>
+        <v>509</v>
+      </c>
+      <c r="E37" s="62" t="s">
+        <v>589</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>11</v>
       </c>
       <c r="G37" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="54"/>
+        <v>473</v>
+      </c>
+      <c r="H37" s="54" t="s">
+        <v>482</v>
+      </c>
+      <c r="I37" s="54" t="s">
+        <v>474</v>
+      </c>
       <c r="K37" s="54"/>
     </row>
     <row r="38" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3754,18 +3763,21 @@
         <v>13</v>
       </c>
       <c r="D38" s="67" t="s">
-        <v>515</v>
-      </c>
-      <c r="E38" s="61" t="s">
-        <v>600</v>
+        <v>543</v>
+      </c>
+      <c r="E38" s="62" t="s">
+        <v>580</v>
       </c>
       <c r="F38" s="54" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="G38" s="54" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="H38" s="54"/>
+      <c r="I38" s="54" t="s">
+        <v>59</v>
+      </c>
       <c r="K38" s="54"/>
     </row>
     <row r="39" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3779,18 +3791,19 @@
         <v>13</v>
       </c>
       <c r="D39" s="67" t="s">
-        <v>516</v>
-      </c>
-      <c r="E39" s="61" t="s">
-        <v>601</v>
+        <v>544</v>
+      </c>
+      <c r="E39" s="69" t="s">
+        <v>627</v>
       </c>
       <c r="F39" s="54" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="G39" s="54" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
       <c r="K39" s="54"/>
     </row>
     <row r="40" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3804,16 +3817,16 @@
         <v>13</v>
       </c>
       <c r="D40" s="67" t="s">
-        <v>517</v>
-      </c>
-      <c r="E40" s="61" t="s">
-        <v>602</v>
+        <v>545</v>
+      </c>
+      <c r="E40" s="69" t="s">
+        <v>628</v>
       </c>
       <c r="F40" s="54" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="G40" s="54" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="H40" s="54"/>
       <c r="K40" s="54"/>
@@ -3829,10 +3842,10 @@
         <v>13</v>
       </c>
       <c r="D41" s="67" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="E41" s="61" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>11</v>
@@ -3854,10 +3867,10 @@
         <v>13</v>
       </c>
       <c r="D42" s="67" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E42" s="61" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>11</v>
@@ -3879,10 +3892,10 @@
         <v>13</v>
       </c>
       <c r="D43" s="67" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="E43" s="61" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>11</v>
@@ -3904,10 +3917,10 @@
         <v>13</v>
       </c>
       <c r="D44" s="67" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="E44" s="61" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>11</v>
@@ -3915,8 +3928,7 @@
       <c r="G44" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54"/>
+      <c r="H44" s="54"/>
       <c r="K44" s="54"/>
     </row>
     <row r="45" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3930,10 +3942,10 @@
         <v>13</v>
       </c>
       <c r="D45" s="67" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="E45" s="61" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>11</v>
@@ -3942,8 +3954,6 @@
         <v>34</v>
       </c>
       <c r="H45" s="54"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="54"/>
       <c r="K45" s="54"/>
     </row>
     <row r="46" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3957,10 +3967,10 @@
         <v>13</v>
       </c>
       <c r="D46" s="67" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="E46" s="61" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>11</v>
@@ -3969,8 +3979,6 @@
         <v>34</v>
       </c>
       <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
       <c r="K46" s="54"/>
     </row>
     <row r="47" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3984,10 +3992,10 @@
         <v>13</v>
       </c>
       <c r="D47" s="67" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="E47" s="61" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>11</v>
@@ -3996,8 +4004,6 @@
         <v>34</v>
       </c>
       <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
       <c r="K47" s="54"/>
     </row>
     <row r="48" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4011,10 +4017,10 @@
         <v>13</v>
       </c>
       <c r="D48" s="67" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E48" s="61" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>11</v>
@@ -4023,8 +4029,6 @@
         <v>34</v>
       </c>
       <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
       <c r="K48" s="54"/>
     </row>
     <row r="49" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4038,10 +4042,10 @@
         <v>13</v>
       </c>
       <c r="D49" s="67" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E49" s="61" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>11</v>
@@ -4049,7 +4053,6 @@
       <c r="G49" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="H49" s="54"/>
       <c r="I49" s="54"/>
       <c r="J49" s="54"/>
       <c r="K49" s="54"/>
@@ -4065,10 +4068,10 @@
         <v>13</v>
       </c>
       <c r="D50" s="67" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E50" s="61" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>11</v>
@@ -4092,10 +4095,10 @@
         <v>13</v>
       </c>
       <c r="D51" s="67" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E51" s="61" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>11</v>
@@ -4119,10 +4122,10 @@
         <v>13</v>
       </c>
       <c r="D52" s="67" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E52" s="61" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="F52" s="54" t="s">
         <v>11</v>
@@ -4146,10 +4149,10 @@
         <v>13</v>
       </c>
       <c r="D53" s="67" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E53" s="61" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F53" s="54" t="s">
         <v>11</v>
@@ -4162,7 +4165,7 @@
       <c r="J53" s="54"/>
       <c r="K53" s="54"/>
     </row>
-    <row r="54" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="55" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="52">
         <v>53</v>
       </c>
@@ -4173,10 +4176,10 @@
         <v>13</v>
       </c>
       <c r="D54" s="67" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E54" s="61" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="F54" s="54" t="s">
         <v>11</v>
@@ -4200,10 +4203,10 @@
         <v>13</v>
       </c>
       <c r="D55" s="67" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E55" s="61" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="F55" s="54" t="s">
         <v>11</v>
@@ -4227,10 +4230,10 @@
         <v>13</v>
       </c>
       <c r="D56" s="67" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E56" s="61" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F56" s="54" t="s">
         <v>11</v>
@@ -4254,10 +4257,10 @@
         <v>13</v>
       </c>
       <c r="D57" s="67" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E57" s="61" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F57" s="54" t="s">
         <v>11</v>
@@ -4281,10 +4284,10 @@
         <v>13</v>
       </c>
       <c r="D58" s="67" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E58" s="61" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F58" s="54" t="s">
         <v>11</v>
@@ -4308,10 +4311,10 @@
         <v>13</v>
       </c>
       <c r="D59" s="67" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E59" s="61" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F59" s="54" t="s">
         <v>11</v>
@@ -4335,10 +4338,10 @@
         <v>13</v>
       </c>
       <c r="D60" s="67" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E60" s="61" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F60" s="54" t="s">
         <v>11</v>
@@ -4362,10 +4365,10 @@
         <v>13</v>
       </c>
       <c r="D61" s="67" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E61" s="63" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F61" s="54" t="s">
         <v>11</v>
@@ -4831,18 +4834,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="55" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
       <c r="B78" s="10"/>
-      <c r="C78" s="56"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="56"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
     </row>
     <row r="79" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="10"/>
@@ -4871,34 +4865,70 @@
     <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="10"/>
       <c r="B85" s="10"/>
+      <c r="C85" s="54"/>
+      <c r="F85" s="54"/>
+      <c r="G85" s="54"/>
+      <c r="H85" s="54"/>
     </row>
     <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="10"/>
-      <c r="B86" s="10"/>
+      <c r="A86" s="52"/>
+      <c r="B86" s="52"/>
+      <c r="C86" s="54"/>
+      <c r="F86" s="54"/>
+      <c r="G86" s="54"/>
+      <c r="H86" s="54"/>
+      <c r="I86" s="54"/>
+      <c r="J86" s="54"/>
     </row>
     <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A87" s="10"/>
-      <c r="B87" s="10"/>
+      <c r="A87" s="52"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="54"/>
+      <c r="F87" s="54"/>
+      <c r="G87" s="54"/>
+      <c r="H87" s="54"/>
+      <c r="I87" s="54"/>
+      <c r="J87" s="54"/>
     </row>
     <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
+      <c r="A88" s="52"/>
+      <c r="B88" s="52"/>
+      <c r="C88" s="54"/>
+      <c r="F88" s="54"/>
+      <c r="G88" s="54"/>
+      <c r="H88" s="54"/>
+      <c r="I88" s="54"/>
+      <c r="J88" s="54"/>
     </row>
     <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="10"/>
-      <c r="B89" s="10"/>
+      <c r="A89" s="52"/>
+      <c r="B89" s="52"/>
+      <c r="C89" s="54"/>
+      <c r="F89" s="54"/>
+      <c r="G89" s="54"/>
+      <c r="H89" s="54"/>
+      <c r="I89" s="54"/>
+      <c r="J89" s="54"/>
     </row>
     <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="10"/>
-      <c r="B90" s="10"/>
+      <c r="A90" s="52"/>
+      <c r="B90" s="52"/>
+      <c r="C90" s="54"/>
+      <c r="F90" s="54"/>
+      <c r="G90" s="54"/>
+      <c r="H90" s="54"/>
+      <c r="I90" s="54"/>
+      <c r="J90" s="54"/>
     </row>
     <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="10"/>
-      <c r="B91" s="10"/>
+      <c r="A91" s="52"/>
+      <c r="B91" s="52"/>
       <c r="C91" s="54"/>
       <c r="F91" s="54"/>
       <c r="G91" s="54"/>
       <c r="H91" s="54"/>
+      <c r="I91" s="54"/>
+      <c r="J91" s="57"/>
     </row>
     <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="52"/>
@@ -4908,145 +4938,127 @@
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
       <c r="I92" s="54"/>
-      <c r="J92" s="54"/>
+      <c r="J92" s="55"/>
     </row>
     <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="52"/>
       <c r="B93" s="52"/>
-      <c r="C93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="54"/>
+      <c r="C93" s="56"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
       <c r="I93" s="54"/>
-      <c r="J93" s="54"/>
+      <c r="J93" s="55"/>
     </row>
     <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="52"/>
-      <c r="B94" s="52"/>
-      <c r="C94" s="54"/>
-      <c r="F94" s="54"/>
-      <c r="G94" s="54"/>
-      <c r="H94" s="54"/>
-      <c r="I94" s="54"/>
-      <c r="J94" s="54"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="9"/>
     </row>
     <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="52"/>
-      <c r="B95" s="52"/>
-      <c r="C95" s="54"/>
-      <c r="F95" s="54"/>
-      <c r="G95" s="54"/>
-      <c r="H95" s="54"/>
-      <c r="I95" s="54"/>
-      <c r="J95" s="54"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="9"/>
     </row>
     <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="52"/>
-      <c r="B96" s="52"/>
-      <c r="C96" s="54"/>
-      <c r="F96" s="54"/>
-      <c r="G96" s="54"/>
-      <c r="H96" s="54"/>
-      <c r="I96" s="54"/>
-      <c r="J96" s="54"/>
-    </row>
-    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A97" s="52"/>
-      <c r="B97" s="52"/>
-      <c r="C97" s="54"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="54"/>
-      <c r="I97" s="54"/>
-      <c r="J97" s="57"/>
-    </row>
-    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="52"/>
-      <c r="B98" s="52"/>
-      <c r="C98" s="54"/>
-      <c r="F98" s="54"/>
-      <c r="G98" s="54"/>
-      <c r="H98" s="54"/>
-      <c r="I98" s="54"/>
-      <c r="J98" s="55"/>
-    </row>
-    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A99" s="52"/>
-      <c r="B99" s="52"/>
-      <c r="C99" s="56"/>
-      <c r="F99" s="29"/>
-      <c r="G99" s="29"/>
-      <c r="H99" s="29"/>
-      <c r="I99" s="54"/>
-      <c r="J99" s="55"/>
-    </row>
-    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A100" s="52"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="9"/>
+    </row>
+    <row r="97" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="10"/>
+      <c r="B97" s="10"/>
+      <c r="C97" s="9"/>
+    </row>
+    <row r="98" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A98" s="10"/>
+      <c r="B98" s="10"/>
+      <c r="C98" s="9"/>
+    </row>
+    <row r="99" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A99" s="10"/>
+      <c r="B99" s="10"/>
+      <c r="C99" s="9"/>
+    </row>
+    <row r="100" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="10"/>
       <c r="B100" s="10"/>
       <c r="C100" s="9"/>
     </row>
-    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="10"/>
       <c r="B101" s="10"/>
       <c r="C101" s="9"/>
     </row>
-    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="10"/>
       <c r="B102" s="10"/>
       <c r="C102" s="9"/>
     </row>
-    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="10"/>
       <c r="B103" s="10"/>
       <c r="C103" s="9"/>
-    </row>
-    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+    </row>
+    <row r="104" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="10"/>
       <c r="B104" s="10"/>
       <c r="C104" s="9"/>
-    </row>
-    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+    </row>
+    <row r="105" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="10"/>
       <c r="B105" s="10"/>
       <c r="C105" s="9"/>
-    </row>
-    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+    </row>
+    <row r="106" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="10"/>
       <c r="B106" s="10"/>
       <c r="C106" s="9"/>
-    </row>
-    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+    </row>
+    <row r="107" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="10"/>
       <c r="B107" s="10"/>
       <c r="C107" s="9"/>
-    </row>
-    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+    </row>
+    <row r="108" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="10"/>
       <c r="B108" s="10"/>
       <c r="C108" s="9"/>
-    </row>
-    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+    </row>
+    <row r="109" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="10"/>
       <c r="B109" s="10"/>
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
     </row>
-    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="10"/>
       <c r="B110" s="10"/>
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
     </row>
-    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="10"/>
       <c r="B111" s="10"/>
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
     </row>
-    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="10"/>
       <c r="B112" s="10"/>
       <c r="C112" s="9"/>
@@ -11321,60 +11333,13 @@
     <row r="1008" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1008" s="10"/>
       <c r="B1008" s="10"/>
-      <c r="C1008" s="9"/>
-      <c r="D1008" s="9"/>
-      <c r="E1008" s="9"/>
-    </row>
-    <row r="1009" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1009" s="10"/>
-      <c r="B1009" s="10"/>
-      <c r="C1009" s="9"/>
-      <c r="D1009" s="9"/>
-      <c r="E1009" s="9"/>
-    </row>
-    <row r="1010" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1010" s="10"/>
-      <c r="B1010" s="10"/>
-      <c r="C1010" s="9"/>
-      <c r="D1010" s="9"/>
-      <c r="E1010" s="9"/>
-    </row>
-    <row r="1011" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1011" s="10"/>
-      <c r="B1011" s="10"/>
-      <c r="C1011" s="9"/>
-      <c r="D1011" s="9"/>
-      <c r="E1011" s="9"/>
-    </row>
-    <row r="1012" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1012" s="10"/>
-      <c r="B1012" s="10"/>
-      <c r="C1012" s="9"/>
-      <c r="D1012" s="9"/>
-      <c r="E1012" s="9"/>
-    </row>
-    <row r="1013" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1013" s="10"/>
-      <c r="B1013" s="10"/>
-      <c r="C1013" s="9"/>
-      <c r="D1013" s="9"/>
-      <c r="E1013" s="9"/>
-    </row>
-    <row r="1014" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1014" s="10"/>
-      <c r="B1014" s="10"/>
-    </row>
-    <row r="1015" spans="1:5" ht="12.75" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="1009" ht="12.75" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:K78" xr:uid="{1E3BF0EA-EC3D-444C-9AE7-3F99453DC04F}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K78">
-      <sortCondition ref="A1:A78"/>
-    </sortState>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K77">
-    <sortCondition ref="B2:B77"/>
-    <sortCondition ref="C2:C77"/>
-    <sortCondition ref="D2:D77"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K1009">
+    <sortCondition ref="B2:B1009"/>
+    <sortCondition ref="C2:C1009"/>
+    <sortCondition ref="D2:D1009"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="J75" r:id="rId1" xr:uid="{3339389E-4D35-4A4F-8174-75A3C203FC63}"/>
@@ -11410,15 +11375,15 @@
     <row r="1" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="73" t="s">
         <v>260</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="72" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="75" t="s">
         <v>261</v>
       </c>
-      <c r="G1" s="71"/>
+      <c r="G1" s="74"/>
     </row>
     <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>

</xml_diff>